<commit_message>
up to 95, testing ALL even more
</commit_message>
<xml_diff>
--- a/testexcel.xlsx
+++ b/testexcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\krisz\bme\szoftech\se-lab4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{29A86EFD-00BC-4777-A2D8-575BE1BB942A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30863E6E-3872-4E6F-ABBB-4AD1298528A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{618B9E70-105F-418C-88FE-DC6B717622DB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{618B9E70-105F-418C-88FE-DC6B717622DB}"/>
   </bookViews>
   <sheets>
     <sheet name="input-0" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="13">
   <si>
     <t>Tesztelt követelmény</t>
   </si>
@@ -73,10 +73,10 @@
     <t>a TORPEDO parancs eredménye FAIL</t>
   </si>
   <si>
-    <t>primary-ben 0, secondaryben 1 torpedo</t>
-  </si>
-  <si>
     <t>primary-ben 4, secondaryben 2 torpedo</t>
+  </si>
+  <si>
+    <t>primary-ben 0, secondaryben 2 torpedo</t>
   </si>
 </sst>
 </file>
@@ -500,10 +500,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08092898-A324-4A8F-BB90-06A010BA41B0}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -525,7 +525,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -613,7 +613,7 @@
         <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -621,6 +621,22 @@
         <v>5</v>
       </c>
       <c r="B20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" t="s">
         <v>10</v>
       </c>
     </row>
@@ -631,10 +647,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE923055-30E1-4423-ADF5-CD42D36B9C37}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -656,7 +672,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -704,6 +720,22 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>